<commit_message>
Fixed typos in filter ids
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/2024_AcidDigestion_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/2024_AcidDigestion_EDI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/GitHub/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B00ADB-4C81-824A-959A-1FE0472077CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A76A90-586A-7948-8920-F89F497CB887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{434214BE-E321-C845-9094-3C530F89F099}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{434214BE-E321-C845-9094-3C530F89F099}"/>
   </bookViews>
   <sheets>
     <sheet name="DigestionA" sheetId="1" r:id="rId1"/>
@@ -683,9 +683,6 @@
     <t>F_sed_8m_R2_F1_05Aug24</t>
   </si>
   <si>
-    <t>B_sed_4m_R2_F1_05Augl24</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_05Aug24</t>
   </si>
   <si>
@@ -767,9 +764,6 @@
     <t>B_sed_4m_R1_F1_19Aug24</t>
   </si>
   <si>
-    <t>B_sed_4m_R2_F1_19Augl24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_19Aug24</t>
   </si>
   <si>
@@ -836,9 +830,6 @@
     <t>B_sed_4m_R1_F1_02Sep24</t>
   </si>
   <si>
-    <t>B_sed_4m_R2_F1_02Sepl24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_02Sep24</t>
   </si>
   <si>
@@ -920,9 +911,6 @@
     <t>B_sed_4m_R1_F1_23Sep24</t>
   </si>
   <si>
-    <t>B_sed_4m_R2_F1_23Sepl24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_23Sep24</t>
   </si>
   <si>
@@ -992,9 +980,6 @@
     <t>B_sed_4m_R1_F1_07Oct24</t>
   </si>
   <si>
-    <t>B_sed_4m_R2_F1_07Octl24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_07Oct24</t>
   </si>
   <si>
@@ -1070,9 +1055,6 @@
     <t>B_sed_4m_R1_F1_21Oct24</t>
   </si>
   <si>
-    <t>B_sed_4m_R2_F1_21Octl24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_21Oct24</t>
   </si>
   <si>
@@ -1154,9 +1136,6 @@
     <t>B_sed_4m_R1_F1_04Nov24</t>
   </si>
   <si>
-    <t>B_sed_4m_R2_F1_04Novl24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_04Nov24</t>
   </si>
   <si>
@@ -1214,9 +1193,6 @@
     <t>B_sed_4m_R1_F1_19Nov24</t>
   </si>
   <si>
-    <t>B_sed_4m_R2_F1_19Novl24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_19Nov24</t>
   </si>
   <si>
@@ -1401,6 +1377,30 @@
   </si>
   <si>
     <t>Duration_days</t>
+  </si>
+  <si>
+    <t>B_sed_4m_R2_F1_05Aug24</t>
+  </si>
+  <si>
+    <t>B_sed_4m_R2_F1_19Aug24</t>
+  </si>
+  <si>
+    <t>B_sed_4m_R2_F1_02Sep24</t>
+  </si>
+  <si>
+    <t>B_sed_4m_R2_F1_23Sep24</t>
+  </si>
+  <si>
+    <t>B_sed_4m_R2_F1_07Oct24</t>
+  </si>
+  <si>
+    <t>B_sed_4m_R2_F1_21Oct24</t>
+  </si>
+  <si>
+    <t>B_sed_4m_R2_F1_04Nov24</t>
+  </si>
+  <si>
+    <t>B_sed_4m_R2_F1_19Nov24</t>
   </si>
 </sst>
 </file>
@@ -1938,14 +1938,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2326,8 +2325,8 @@
   </sheetPr>
   <dimension ref="A1:L155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2362,16 +2361,16 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2404,7 +2403,7 @@
       <c r="K2" s="2">
         <v>0.01</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2438,7 +2437,7 @@
       <c r="K3" s="2">
         <v>0.01</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2472,7 +2471,7 @@
       <c r="K4" s="2">
         <v>0.01</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2506,7 +2505,7 @@
       <c r="K5" s="2">
         <v>0.01</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2540,7 +2539,7 @@
       <c r="K6" s="2">
         <v>0.01</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2574,7 +2573,7 @@
       <c r="K7" s="2">
         <v>0.01</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2608,7 +2607,7 @@
       <c r="K8" s="2">
         <v>0.01</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2642,7 +2641,7 @@
       <c r="K9" s="2">
         <v>0.01</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2676,7 +2675,7 @@
       <c r="K10" s="2">
         <v>0.01</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2710,7 +2709,7 @@
       <c r="K11" s="2">
         <v>0.01</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2744,7 +2743,7 @@
       <c r="K12" s="2">
         <v>0.01</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2778,7 +2777,7 @@
       <c r="K13" s="2">
         <v>0.01</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2812,7 +2811,7 @@
       <c r="K14" s="2">
         <v>0.01</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2846,7 +2845,7 @@
       <c r="K15" s="2">
         <v>0.01</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2880,7 +2879,7 @@
       <c r="K16" s="2">
         <v>0.01</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2914,7 +2913,7 @@
       <c r="K17" s="2">
         <v>0.01</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2948,7 +2947,7 @@
       <c r="K18" s="2">
         <v>0.01</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2982,7 +2981,7 @@
       <c r="K19" s="2">
         <v>0.01</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3016,7 +3015,7 @@
       <c r="K20" s="2">
         <v>0.01</v>
       </c>
-      <c r="L20" s="5">
+      <c r="L20" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3050,7 +3049,7 @@
       <c r="K21" s="2">
         <v>0.01</v>
       </c>
-      <c r="L21" s="5">
+      <c r="L21" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3084,7 +3083,7 @@
       <c r="K22" s="2">
         <v>0.01</v>
       </c>
-      <c r="L22" s="5">
+      <c r="L22" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3118,7 +3117,7 @@
       <c r="K23" s="2">
         <v>0.01</v>
       </c>
-      <c r="L23" s="5">
+      <c r="L23" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3152,7 +3151,7 @@
       <c r="K24" s="2">
         <v>0.01</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L24" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3186,7 +3185,7 @@
       <c r="K25" s="2">
         <v>0.01</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L25" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3220,7 +3219,7 @@
       <c r="K26" s="2">
         <v>0.01</v>
       </c>
-      <c r="L26" s="5">
+      <c r="L26" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3254,7 +3253,7 @@
       <c r="K27" s="2">
         <v>0.01</v>
       </c>
-      <c r="L27" s="5">
+      <c r="L27" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3288,7 +3287,7 @@
       <c r="K28" s="2">
         <v>0.01</v>
       </c>
-      <c r="L28" s="5">
+      <c r="L28" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3322,7 +3321,7 @@
       <c r="K29" s="2">
         <v>0.01</v>
       </c>
-      <c r="L29" s="5">
+      <c r="L29" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3356,7 +3355,7 @@
       <c r="K30" s="2">
         <v>0.01</v>
       </c>
-      <c r="L30" s="5">
+      <c r="L30" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3390,7 +3389,7 @@
       <c r="K31" s="2">
         <v>0.01</v>
       </c>
-      <c r="L31" s="5">
+      <c r="L31" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3424,7 +3423,7 @@
       <c r="K32" s="2">
         <v>0.01</v>
       </c>
-      <c r="L32" s="5">
+      <c r="L32" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3458,7 +3457,7 @@
       <c r="K33" s="2">
         <v>0.01</v>
       </c>
-      <c r="L33" s="5">
+      <c r="L33" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3492,7 +3491,7 @@
       <c r="K34" s="2">
         <v>0.01</v>
       </c>
-      <c r="L34" s="5">
+      <c r="L34" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3526,7 +3525,7 @@
       <c r="K35" s="2">
         <v>0.01</v>
       </c>
-      <c r="L35" s="5">
+      <c r="L35" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3560,7 +3559,7 @@
       <c r="K36" s="2">
         <v>0.01</v>
       </c>
-      <c r="L36" s="5">
+      <c r="L36" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3594,7 +3593,7 @@
       <c r="K37" s="2">
         <v>0.01</v>
       </c>
-      <c r="L37" s="5">
+      <c r="L37" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3628,7 +3627,7 @@
       <c r="K38" s="2">
         <v>0.01</v>
       </c>
-      <c r="L38" s="5">
+      <c r="L38" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3662,7 +3661,7 @@
       <c r="K39" s="2">
         <v>0.01</v>
       </c>
-      <c r="L39" s="5">
+      <c r="L39" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3692,7 +3691,7 @@
       <c r="K40" s="2">
         <v>0.01</v>
       </c>
-      <c r="L40" s="5"/>
+      <c r="L40" s="4"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
@@ -3718,7 +3717,7 @@
       <c r="K41" s="2">
         <v>0.01</v>
       </c>
-      <c r="L41" s="5"/>
+      <c r="L41" s="4"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
@@ -3750,7 +3749,7 @@
       <c r="K42" s="2">
         <v>0.01</v>
       </c>
-      <c r="L42" s="5">
+      <c r="L42" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3784,7 +3783,7 @@
       <c r="K43" s="2">
         <v>0.01</v>
       </c>
-      <c r="L43" s="5">
+      <c r="L43" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3818,7 +3817,7 @@
       <c r="K44" s="2">
         <v>0.01</v>
       </c>
-      <c r="L44" s="5">
+      <c r="L44" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3852,7 +3851,7 @@
       <c r="K45" s="2">
         <v>0.01</v>
       </c>
-      <c r="L45" s="5">
+      <c r="L45" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3886,7 +3885,7 @@
       <c r="K46" s="2">
         <v>0.01</v>
       </c>
-      <c r="L46" s="5">
+      <c r="L46" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3920,7 +3919,7 @@
       <c r="K47" s="2">
         <v>0.01</v>
       </c>
-      <c r="L47" s="5">
+      <c r="L47" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3954,7 +3953,7 @@
       <c r="K48" s="2">
         <v>0.01</v>
       </c>
-      <c r="L48" s="5">
+      <c r="L48" s="4">
         <v>14</v>
       </c>
     </row>
@@ -3988,7 +3987,7 @@
       <c r="K49" s="2">
         <v>0.01</v>
       </c>
-      <c r="L49" s="5">
+      <c r="L49" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4022,7 +4021,7 @@
       <c r="K50" s="2">
         <v>0.01</v>
       </c>
-      <c r="L50" s="5">
+      <c r="L50" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4056,7 +4055,7 @@
       <c r="K51" s="2">
         <v>0.01</v>
       </c>
-      <c r="L51" s="5">
+      <c r="L51" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4090,7 +4089,7 @@
       <c r="K52" s="2">
         <v>0.01</v>
       </c>
-      <c r="L52" s="5">
+      <c r="L52" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4124,7 +4123,7 @@
       <c r="K53" s="2">
         <v>0.01</v>
       </c>
-      <c r="L53" s="5">
+      <c r="L53" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4158,7 +4157,7 @@
       <c r="K54" s="2">
         <v>0.01</v>
       </c>
-      <c r="L54" s="5">
+      <c r="L54" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4192,7 +4191,7 @@
       <c r="K55" s="2">
         <v>0.01</v>
       </c>
-      <c r="L55" s="5">
+      <c r="L55" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4226,7 +4225,7 @@
       <c r="K56" s="2">
         <v>0.01</v>
       </c>
-      <c r="L56" s="5">
+      <c r="L56" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4260,7 +4259,7 @@
       <c r="K57" s="2">
         <v>0.01</v>
       </c>
-      <c r="L57" s="5">
+      <c r="L57" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4294,7 +4293,7 @@
       <c r="K58" s="2">
         <v>0.01</v>
       </c>
-      <c r="L58" s="5">
+      <c r="L58" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4328,7 +4327,7 @@
       <c r="K59" s="2">
         <v>0.01</v>
       </c>
-      <c r="L59" s="5">
+      <c r="L59" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4362,7 +4361,7 @@
       <c r="K60" s="2">
         <v>0.01</v>
       </c>
-      <c r="L60" s="5">
+      <c r="L60" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4396,7 +4395,7 @@
       <c r="K61" s="2">
         <v>0.01</v>
       </c>
-      <c r="L61" s="5">
+      <c r="L61" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4430,7 +4429,7 @@
       <c r="K62" s="2">
         <v>0.01</v>
       </c>
-      <c r="L62" s="5">
+      <c r="L62" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4464,7 +4463,7 @@
       <c r="K63" s="2">
         <v>0.01</v>
       </c>
-      <c r="L63" s="5">
+      <c r="L63" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4498,7 +4497,7 @@
       <c r="K64" s="2">
         <v>0.01</v>
       </c>
-      <c r="L64" s="5">
+      <c r="L64" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4532,7 +4531,7 @@
       <c r="K65" s="2">
         <v>0.01</v>
       </c>
-      <c r="L65" s="5">
+      <c r="L65" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4566,7 +4565,7 @@
       <c r="K66" s="2">
         <v>0.01</v>
       </c>
-      <c r="L66" s="5">
+      <c r="L66" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4600,7 +4599,7 @@
       <c r="K67" s="2">
         <v>0.01</v>
       </c>
-      <c r="L67" s="5">
+      <c r="L67" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4612,7 +4611,7 @@
         <v>212</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -4634,7 +4633,7 @@
       <c r="K68" s="2">
         <v>0.01</v>
       </c>
-      <c r="L68" s="5">
+      <c r="L68" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4646,7 +4645,7 @@
         <v>213</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -4668,7 +4667,7 @@
       <c r="K69" s="2">
         <v>0.01</v>
       </c>
-      <c r="L69" s="5">
+      <c r="L69" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4680,7 +4679,7 @@
         <v>214</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -4702,7 +4701,7 @@
       <c r="K70" s="2">
         <v>0.01</v>
       </c>
-      <c r="L70" s="5">
+      <c r="L70" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4714,7 +4713,7 @@
         <v>215</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -4736,7 +4735,7 @@
       <c r="K71" s="2">
         <v>0.01</v>
       </c>
-      <c r="L71" s="5">
+      <c r="L71" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4745,10 +4744,10 @@
         <v>208</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -4770,7 +4769,7 @@
       <c r="K72" s="2">
         <v>0.01</v>
       </c>
-      <c r="L72" s="5">
+      <c r="L72" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4779,10 +4778,10 @@
         <v>209</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>216</v>
+        <v>448</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -4804,7 +4803,7 @@
       <c r="K73" s="2">
         <v>0.01</v>
       </c>
-      <c r="L73" s="5">
+      <c r="L73" s="4">
         <v>14</v>
       </c>
     </row>
@@ -4813,10 +4812,10 @@
         <v>210</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -4838,13 +4837,13 @@
       <c r="K74" s="2">
         <v>0.01</v>
       </c>
-      <c r="L74" s="5">
+      <c r="L74" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>126</v>
@@ -4868,11 +4867,11 @@
       <c r="K75" s="2">
         <v>0.01</v>
       </c>
-      <c r="L75" s="5"/>
+      <c r="L75" s="4"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>127</v>
@@ -4893,17 +4892,17 @@
       <c r="K76" s="2">
         <v>0.01</v>
       </c>
-      <c r="L76" s="5"/>
+      <c r="L76" s="4"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>211</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -4925,19 +4924,19 @@
       <c r="K77" s="2">
         <v>0.01</v>
       </c>
-      <c r="L77" s="5">
+      <c r="L77" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -4959,19 +4958,19 @@
       <c r="K78" s="2">
         <v>0.01</v>
       </c>
-      <c r="L78" s="5">
+      <c r="L78" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -4993,19 +4992,19 @@
       <c r="K79" s="2">
         <v>0.01</v>
       </c>
-      <c r="L79" s="5">
+      <c r="L79" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -5027,19 +5026,19 @@
       <c r="K80" s="2">
         <v>0.01</v>
       </c>
-      <c r="L80" s="5">
+      <c r="L80" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -5061,19 +5060,19 @@
       <c r="K81" s="2">
         <v>0.01</v>
       </c>
-      <c r="L81" s="5">
+      <c r="L81" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -5095,19 +5094,19 @@
       <c r="K82" s="2">
         <v>0.01</v>
       </c>
-      <c r="L82" s="5">
+      <c r="L82" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>244</v>
+        <v>449</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -5129,19 +5128,19 @@
       <c r="K83" s="2">
         <v>0.01</v>
       </c>
-      <c r="L83" s="5">
+      <c r="L83" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -5163,19 +5162,19 @@
       <c r="K84" s="2">
         <v>0.01</v>
       </c>
-      <c r="L84" s="5">
+      <c r="L84" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="C85" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -5197,19 +5196,19 @@
       <c r="K85" s="2">
         <v>0.01</v>
       </c>
-      <c r="L85" s="5">
+      <c r="L85" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -5231,19 +5230,19 @@
       <c r="K86" s="2">
         <v>0.01</v>
       </c>
-      <c r="L86" s="5">
+      <c r="L86" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -5265,19 +5264,19 @@
       <c r="K87" s="2">
         <v>0.01</v>
       </c>
-      <c r="L87" s="5">
+      <c r="L87" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -5299,19 +5298,19 @@
       <c r="K88" s="2">
         <v>0.01</v>
       </c>
-      <c r="L88" s="5">
+      <c r="L88" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -5333,19 +5332,19 @@
       <c r="K89" s="2">
         <v>0.01</v>
       </c>
-      <c r="L89" s="5">
+      <c r="L89" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -5367,19 +5366,19 @@
       <c r="K90" s="2">
         <v>0.01</v>
       </c>
-      <c r="L90" s="5">
+      <c r="L90" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>267</v>
+        <v>450</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
@@ -5401,19 +5400,19 @@
       <c r="K91" s="2">
         <v>0.01</v>
       </c>
-      <c r="L91" s="5">
+      <c r="L91" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -5435,19 +5434,19 @@
       <c r="K92" s="2">
         <v>0.01</v>
       </c>
-      <c r="L92" s="5">
+      <c r="L92" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -5469,19 +5468,19 @@
       <c r="K93" s="2">
         <v>0.01</v>
       </c>
-      <c r="L93" s="5">
+      <c r="L93" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -5503,19 +5502,19 @@
       <c r="K94" s="2">
         <v>0.01</v>
       </c>
-      <c r="L94" s="5">
+      <c r="L94" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -5537,19 +5536,19 @@
       <c r="K95" s="2">
         <v>0.01</v>
       </c>
-      <c r="L95" s="5">
+      <c r="L95" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -5571,19 +5570,19 @@
       <c r="K96" s="2">
         <v>0.01</v>
       </c>
-      <c r="L96" s="5">
+      <c r="L96" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -5605,19 +5604,19 @@
       <c r="K97" s="2">
         <v>0.01</v>
       </c>
-      <c r="L97" s="5">
+      <c r="L97" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -5639,19 +5638,19 @@
       <c r="K98" s="2">
         <v>0.01</v>
       </c>
-      <c r="L98" s="5">
+      <c r="L98" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>295</v>
+        <v>451</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -5673,19 +5672,19 @@
       <c r="K99" s="2">
         <v>0.01</v>
       </c>
-      <c r="L99" s="5">
+      <c r="L99" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -5707,19 +5706,19 @@
       <c r="K100" s="2">
         <v>0.01</v>
       </c>
-      <c r="L100" s="5">
+      <c r="L100" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -5741,19 +5740,19 @@
       <c r="K101" s="2">
         <v>0.01</v>
       </c>
-      <c r="L101" s="5">
+      <c r="L101" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -5775,19 +5774,19 @@
       <c r="K102" s="2">
         <v>0.01</v>
       </c>
-      <c r="L102" s="5">
+      <c r="L102" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -5809,19 +5808,19 @@
       <c r="K103" s="2">
         <v>0.01</v>
       </c>
-      <c r="L103" s="5">
+      <c r="L103" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -5843,19 +5842,19 @@
       <c r="K104" s="2">
         <v>0.01</v>
       </c>
-      <c r="L104" s="5">
+      <c r="L104" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>313</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
@@ -5877,19 +5876,19 @@
       <c r="K105" s="2">
         <v>0.01</v>
       </c>
-      <c r="L105" s="5">
+      <c r="L105" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="C106" s="2" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
@@ -5911,19 +5910,19 @@
       <c r="K106" s="2">
         <v>0.01</v>
       </c>
-      <c r="L106" s="5">
+      <c r="L106" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>319</v>
+        <v>452</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
@@ -5945,19 +5944,19 @@
       <c r="K107" s="2">
         <v>0.01</v>
       </c>
-      <c r="L107" s="5">
+      <c r="L107" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
@@ -5979,19 +5978,19 @@
       <c r="K108" s="2">
         <v>0.01</v>
       </c>
-      <c r="L108" s="5">
+      <c r="L108" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
@@ -6013,19 +6012,19 @@
       <c r="K109" s="2">
         <v>0.01</v>
       </c>
-      <c r="L109" s="5">
+      <c r="L109" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
@@ -6047,19 +6046,19 @@
       <c r="K110" s="2">
         <v>0.01</v>
       </c>
-      <c r="L110" s="5">
+      <c r="L110" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
@@ -6081,19 +6080,19 @@
       <c r="K111" s="2">
         <v>0.01</v>
       </c>
-      <c r="L111" s="5">
+      <c r="L111" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
@@ -6115,19 +6114,19 @@
       <c r="K112" s="2">
         <v>0.01</v>
       </c>
-      <c r="L112" s="5">
+      <c r="L112" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
@@ -6149,13 +6148,13 @@
       <c r="K113" s="2">
         <v>0.01</v>
       </c>
-      <c r="L113" s="5">
+      <c r="L113" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>126</v>
@@ -6179,13 +6178,13 @@
       <c r="K114" s="2">
         <v>0.01</v>
       </c>
-      <c r="L114" s="5">
+      <c r="L114" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>127</v>
@@ -6207,19 +6206,19 @@
       <c r="K115" s="2">
         <v>0.01</v>
       </c>
-      <c r="L115" s="5">
+      <c r="L115" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
@@ -6241,19 +6240,19 @@
       <c r="K116" s="2">
         <v>0.01</v>
       </c>
-      <c r="L116" s="5">
+      <c r="L116" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>345</v>
+        <v>453</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
@@ -6275,19 +6274,19 @@
       <c r="K117" s="2">
         <v>0.01</v>
       </c>
-      <c r="L117" s="5">
+      <c r="L117" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
@@ -6309,19 +6308,19 @@
       <c r="K118" s="2">
         <v>0.01</v>
       </c>
-      <c r="L118" s="5">
+      <c r="L118" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
@@ -6343,19 +6342,19 @@
       <c r="K119" s="2">
         <v>0.01</v>
       </c>
-      <c r="L119" s="5">
+      <c r="L119" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
@@ -6377,19 +6376,19 @@
       <c r="K120" s="2">
         <v>0.01</v>
       </c>
-      <c r="L120" s="5">
+      <c r="L120" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
@@ -6411,19 +6410,19 @@
       <c r="K121" s="2">
         <v>0.01</v>
       </c>
-      <c r="L121" s="5">
+      <c r="L121" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
@@ -6445,19 +6444,19 @@
       <c r="K122" s="2">
         <v>0.01</v>
       </c>
-      <c r="L122" s="5">
+      <c r="L122" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
@@ -6479,19 +6478,19 @@
       <c r="K123" s="2">
         <v>0.01</v>
       </c>
-      <c r="L123" s="5">
+      <c r="L123" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
@@ -6513,19 +6512,19 @@
       <c r="K124" s="2">
         <v>0.01</v>
       </c>
-      <c r="L124" s="5">
+      <c r="L124" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>373</v>
+        <v>454</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
@@ -6547,19 +6546,19 @@
       <c r="K125" s="2">
         <v>0.01</v>
       </c>
-      <c r="L125" s="5">
+      <c r="L125" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
@@ -6581,19 +6580,19 @@
       <c r="K126" s="2">
         <v>0.01</v>
       </c>
-      <c r="L126" s="5">
+      <c r="L126" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
@@ -6615,19 +6614,19 @@
       <c r="K127" s="2">
         <v>0.01</v>
       </c>
-      <c r="L127" s="5">
+      <c r="L127" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
@@ -6649,19 +6648,19 @@
       <c r="K128" s="2">
         <v>0.01</v>
       </c>
-      <c r="L128" s="5">
+      <c r="L128" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
@@ -6683,19 +6682,19 @@
       <c r="K129" s="2">
         <v>0.01</v>
       </c>
-      <c r="L129" s="5">
+      <c r="L129" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
@@ -6717,19 +6716,19 @@
       <c r="K130" s="2">
         <v>0.01</v>
       </c>
-      <c r="L130" s="5">
+      <c r="L130" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
@@ -6751,19 +6750,19 @@
       <c r="K131" s="2">
         <v>0.01</v>
       </c>
-      <c r="L131" s="5">
+      <c r="L131" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>396</v>
       </c>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
@@ -6785,19 +6784,19 @@
       <c r="K132" s="2">
         <v>0.01</v>
       </c>
-      <c r="L132" s="5">
+      <c r="L132" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C133" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>397</v>
       </c>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
@@ -6819,19 +6818,19 @@
       <c r="K133" s="2">
         <v>0.01</v>
       </c>
-      <c r="L133" s="5">
+      <c r="L133" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C134" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>398</v>
       </c>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
@@ -6853,19 +6852,19 @@
       <c r="K134" s="2">
         <v>0.01</v>
       </c>
-      <c r="L134" s="5">
+      <c r="L134" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>399</v>
       </c>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
@@ -6887,13 +6886,13 @@
       <c r="K135" s="2">
         <v>0.01</v>
       </c>
-      <c r="L135" s="5">
+      <c r="L135" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>126</v>
@@ -6920,7 +6919,7 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>127</v>
@@ -6945,13 +6944,13 @@
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="C138" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>418</v>
       </c>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
@@ -6973,19 +6972,19 @@
       <c r="K138" s="2">
         <v>0.01</v>
       </c>
-      <c r="L138" s="5">
+      <c r="L138" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="C139" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>419</v>
       </c>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
@@ -7007,19 +7006,19 @@
       <c r="K139" s="2">
         <v>0.01</v>
       </c>
-      <c r="L139" s="6">
+      <c r="L139" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="C140" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
@@ -7041,19 +7040,19 @@
       <c r="K140" s="2">
         <v>0.01</v>
       </c>
-      <c r="L140" s="6">
+      <c r="L140" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="C141" s="2" t="s">
         <v>413</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>421</v>
       </c>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
@@ -7075,19 +7074,19 @@
       <c r="K141" s="2">
         <v>0.01</v>
       </c>
-      <c r="L141" s="6">
+      <c r="L141" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="C142" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>422</v>
       </c>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
@@ -7109,19 +7108,19 @@
       <c r="K142" s="2">
         <v>0.01</v>
       </c>
-      <c r="L142" s="6">
+      <c r="L142" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="C143" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>423</v>
       </c>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
@@ -7143,19 +7142,19 @@
       <c r="K143" s="2">
         <v>0.01</v>
       </c>
-      <c r="L143" s="6">
+      <c r="L143" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="C144" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>424</v>
       </c>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
@@ -7177,19 +7176,19 @@
       <c r="K144" s="2">
         <v>0.01</v>
       </c>
-      <c r="L144" s="6">
+      <c r="L144" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="C145" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
@@ -7211,19 +7210,19 @@
       <c r="K145" s="2">
         <v>0.01</v>
       </c>
-      <c r="L145" s="6">
+      <c r="L145" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="C146" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>442</v>
       </c>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
@@ -7245,19 +7244,19 @@
       <c r="K146" s="2">
         <v>0.01</v>
       </c>
-      <c r="L146" s="6">
+      <c r="L146" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="C147" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
@@ -7279,19 +7278,19 @@
       <c r="K147" s="2">
         <v>0.01</v>
       </c>
-      <c r="L147" s="6">
+      <c r="L147" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>444</v>
       </c>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
@@ -7313,19 +7312,19 @@
       <c r="K148" s="2">
         <v>0.01</v>
       </c>
-      <c r="L148" s="6">
+      <c r="L148" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="C149" s="2" t="s">
         <v>437</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>445</v>
       </c>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
@@ -7347,19 +7346,19 @@
       <c r="K149" s="2">
         <v>0.01</v>
       </c>
-      <c r="L149" s="6">
+      <c r="L149" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B150" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="C150" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>446</v>
       </c>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
@@ -7381,19 +7380,19 @@
       <c r="K150" s="2">
         <v>0.01</v>
       </c>
-      <c r="L150" s="6">
+      <c r="L150" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="C151" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>447</v>
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
@@ -7415,19 +7414,19 @@
       <c r="K151" s="2">
         <v>0.01</v>
       </c>
-      <c r="L151" s="6">
+      <c r="L151" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>448</v>
       </c>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
@@ -7449,19 +7448,19 @@
       <c r="K152" s="2">
         <v>0.01</v>
       </c>
-      <c r="L152" s="6">
+      <c r="L152" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="C153" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>449</v>
       </c>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
@@ -7483,13 +7482,13 @@
       <c r="K153" s="2">
         <v>0.01</v>
       </c>
-      <c r="L153" s="6">
+      <c r="L153" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>126</v>
@@ -7513,11 +7512,11 @@
       <c r="K154" s="2">
         <v>0.01</v>
       </c>
-      <c r="L154" s="6"/>
+      <c r="L154" s="5"/>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>127</v>
@@ -7539,7 +7538,7 @@
       <c r="K155" s="2">
         <v>0.01</v>
       </c>
-      <c r="L155" s="6"/>
+      <c r="L155" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>